<commit_message>
update schedule and access info
</commit_message>
<xml_diff>
--- a/public/people/SCmemberList.xlsx
+++ b/public/people/SCmemberList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masudasatoki/Desktop/tristan2025-website/content/people/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373AB0FC-F19D-CA49-9F02-681367FBF938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCA3975-4853-5D48-AB1D-A93E38FD6BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$132</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="403">
   <si>
     <t>Name</t>
   </si>
@@ -953,9 +953,6 @@
     <t>University of Liverpool</t>
   </si>
   <si>
-    <t>Heudiasyc</t>
-  </si>
-  <si>
     <t>University of Hamburg</t>
   </si>
   <si>
@@ -1130,6 +1127,173 @@
   <si>
     <t>Rui Yao</t>
     <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>IMT Atlantique</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Rotterdam School of Management</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>Lei Zhao</t>
+  </si>
+  <si>
+    <t>Angelica Del Rocio Lozano Cuevas</t>
+  </si>
+  <si>
+    <t>Stefan Minner</t>
+  </si>
+  <si>
+    <t>Mihaela Popa</t>
+  </si>
+  <si>
+    <t>Ruibin Bai</t>
+  </si>
+  <si>
+    <t>Richard Wong</t>
+  </si>
+  <si>
+    <t>Nadia Lahrichi</t>
+  </si>
+  <si>
+    <t>Kjetil Fagerholt</t>
+  </si>
+  <si>
+    <t>Norwegian University of Science and Technology</t>
+  </si>
+  <si>
+    <t>Jorge Mendoza Gimenez</t>
+  </si>
+  <si>
+    <t>Fausto Errico</t>
+  </si>
+  <si>
+    <t>CIRRELT and École de technologie supérieure de Montréal</t>
+  </si>
+  <si>
+    <t>Guido Perboli</t>
+  </si>
+  <si>
+    <t>Politecnico di Torino, Italy and CIRRELT, Canada</t>
+  </si>
+  <si>
+    <t>Federico Malucelli</t>
+  </si>
+  <si>
+    <t>Politecnico di Milano</t>
+  </si>
+  <si>
+    <t>Massimo Di Francesco</t>
+  </si>
+  <si>
+    <t>Manuel Iori</t>
+  </si>
+  <si>
+    <t>University of Modena and Reggio Emilia</t>
+  </si>
+  <si>
+    <t>Antonio Frangioni</t>
+  </si>
+  <si>
+    <t>Maria Elena Bruni</t>
+  </si>
+  <si>
+    <t>University of Calabria</t>
+  </si>
+  <si>
+    <t>Tsinghua University</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Universidad Nacional Autónoma de México	</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Panagiotis Repoussis</t>
+  </si>
+  <si>
+    <t>Athens University of Economics and Business</t>
+  </si>
+  <si>
+    <t>Alexandre Jacquillat</t>
+  </si>
+  <si>
+    <t>Massachusetts Institute of Technology</t>
+  </si>
+  <si>
+    <t>Anne Goodchild</t>
+  </si>
+  <si>
+    <t>Ann Melissa Campbell</t>
+  </si>
+  <si>
+    <t>University of Iowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical University of Munich	</t>
+  </si>
+  <si>
+    <t>University Politehnica of Bucharest</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>University of Nottingham Ningbo</t>
+  </si>
+  <si>
+    <t>Anant Balakrishnan</t>
+  </si>
+  <si>
+    <t>University of Texas</t>
+  </si>
+  <si>
+    <t>Antonio Mauttone</t>
+  </si>
+  <si>
+    <t>Universidad de la República</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Claudio Sterle</t>
+  </si>
+  <si>
+    <t>University of Naples</t>
+  </si>
+  <si>
+    <t>Margaretha Gansterer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Vienna	</t>
+  </si>
+  <si>
+    <t>Karl F. Doerner</t>
+  </si>
+  <si>
+    <t>Leandro Callegari Coelho</t>
+  </si>
+  <si>
+    <t>Polytechnique Montréal</t>
+  </si>
+  <si>
+    <t>Università di Cagliari</t>
+  </si>
+  <si>
+    <t>Università di Pisa</t>
+  </si>
+  <si>
+    <t>Gianfranco Guastaroba</t>
+  </si>
+  <si>
+    <t>Bilge Atasoy</t>
   </si>
 </sst>
 </file>
@@ -1613,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="125" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="B176" sqref="B176"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="125" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="D189" sqref="D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="20"/>
@@ -1798,7 +1962,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C14" t="s">
         <v>191</v>
@@ -2994,7 +3158,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>297</v>
+        <v>348</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>227</v>
@@ -3020,7 +3184,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C108" s="12" t="s">
         <v>237</v>
@@ -3059,7 +3223,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C111" s="12" t="s">
         <v>225</v>
@@ -3085,7 +3249,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>227</v>
@@ -3098,7 +3262,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C114" s="12" t="s">
         <v>225</v>
@@ -3111,7 +3275,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C115" s="12" t="s">
         <v>227</v>
@@ -3124,7 +3288,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C116" s="12" t="s">
         <v>225</v>
@@ -3150,7 +3314,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C118" s="12" t="s">
         <v>225</v>
@@ -3163,7 +3327,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C119" s="12" t="s">
         <v>250</v>
@@ -3241,7 +3405,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>241</v>
@@ -3254,7 +3418,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C126" s="12" t="s">
         <v>227</v>
@@ -3306,7 +3470,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C130" s="12" t="s">
         <v>254</v>
@@ -3345,7 +3509,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C133" s="12" t="s">
         <v>187</v>
@@ -3371,7 +3535,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C135" t="s">
         <v>191</v>
@@ -3436,10 +3600,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
+        <v>312</v>
+      </c>
+      <c r="C140" t="s">
         <v>313</v>
-      </c>
-      <c r="C140" t="s">
-        <v>314</v>
       </c>
       <c r="D140" s="12"/>
       <c r="E140" s="12"/>
@@ -3475,7 +3639,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C143" t="s">
         <v>191</v>
@@ -3501,7 +3665,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C145" t="s">
         <v>191</v>
@@ -3514,7 +3678,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C146" t="s">
         <v>191</v>
@@ -3527,7 +3691,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C147" t="s">
         <v>191</v>
@@ -3540,7 +3704,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>227</v>
@@ -3566,10 +3730,10 @@
         <v>149</v>
       </c>
       <c r="B150" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="C150" s="12" t="s">
         <v>310</v>
-      </c>
-      <c r="C150" s="12" t="s">
-        <v>311</v>
       </c>
       <c r="D150" s="12"/>
       <c r="E150" s="12"/>
@@ -3579,7 +3743,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C151" s="12" t="s">
         <v>247</v>
@@ -3629,7 +3793,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C155" s="12" t="s">
         <v>254</v>
@@ -3655,7 +3819,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C157" s="12" t="s">
         <v>225</v>
@@ -3694,7 +3858,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C160" s="12" t="s">
         <v>250</v>
@@ -3707,10 +3871,10 @@
         <v>160</v>
       </c>
       <c r="B161" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C161" s="12" t="s">
         <v>318</v>
-      </c>
-      <c r="C161" s="12" t="s">
-        <v>319</v>
       </c>
       <c r="D161" s="12"/>
       <c r="E161" s="12"/>
@@ -3720,7 +3884,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C162" s="12" t="s">
         <v>237</v>
@@ -3759,7 +3923,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="12" t="s">
-        <v>228</v>
+        <v>349</v>
       </c>
       <c r="C165" s="12" t="s">
         <v>229</v>
@@ -3772,7 +3936,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C166" s="12" t="s">
         <v>225</v>
@@ -3785,7 +3949,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C167" s="12" t="s">
         <v>229</v>
@@ -3798,10 +3962,10 @@
         <v>167</v>
       </c>
       <c r="B168" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C168" s="12" t="s">
         <v>322</v>
-      </c>
-      <c r="C168" s="12" t="s">
-        <v>323</v>
       </c>
       <c r="D168" s="12"/>
       <c r="E168" s="12"/>
@@ -3860,21 +4024,21 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" t="s">
+        <v>329</v>
+      </c>
+      <c r="B173" t="s">
+        <v>331</v>
+      </c>
+      <c r="C173" s="12" t="s">
         <v>330</v>
-      </c>
-      <c r="B173" t="s">
-        <v>332</v>
-      </c>
-      <c r="C173" s="12" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="174" spans="1:5">
       <c r="A174" t="s">
+        <v>332</v>
+      </c>
+      <c r="B174" t="s">
         <v>333</v>
-      </c>
-      <c r="B174" t="s">
-        <v>334</v>
       </c>
       <c r="C174" s="11" t="s">
         <v>191</v>
@@ -3882,10 +4046,10 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" t="s">
+        <v>334</v>
+      </c>
+      <c r="B175" t="s">
         <v>335</v>
-      </c>
-      <c r="B175" t="s">
-        <v>336</v>
       </c>
       <c r="C175" s="11" t="s">
         <v>191</v>
@@ -3893,10 +4057,10 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B176" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C176" s="11" t="s">
         <v>191</v>
@@ -3904,7 +4068,7 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B177" t="s">
         <v>213</v>
@@ -3915,7 +4079,7 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B178" t="s">
         <v>202</v>
@@ -3926,29 +4090,29 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
+        <v>340</v>
+      </c>
+      <c r="B179" t="s">
         <v>341</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" s="11" t="s">
         <v>342</v>
-      </c>
-      <c r="C179" s="11" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
+        <v>343</v>
+      </c>
+      <c r="B180" t="s">
         <v>344</v>
       </c>
-      <c r="B180" t="s">
+      <c r="C180" s="11" t="s">
         <v>345</v>
-      </c>
-      <c r="C180" s="11" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B181" s="12" t="s">
         <v>230</v>
@@ -3959,13 +4123,312 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B182" s="12" t="s">
         <v>230</v>
       </c>
       <c r="C182" s="12" t="s">
         <v>231</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" t="s">
+        <v>350</v>
+      </c>
+      <c r="B183" t="s">
+        <v>372</v>
+      </c>
+      <c r="C183" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" t="s">
+        <v>351</v>
+      </c>
+      <c r="B184" t="s">
+        <v>374</v>
+      </c>
+      <c r="C184" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" t="s">
+        <v>376</v>
+      </c>
+      <c r="B185" t="s">
+        <v>377</v>
+      </c>
+      <c r="C185" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" t="s">
+        <v>378</v>
+      </c>
+      <c r="B186" t="s">
+        <v>379</v>
+      </c>
+      <c r="C186" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>380</v>
+      </c>
+      <c r="B187" t="s">
+        <v>302</v>
+      </c>
+      <c r="C187" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="s">
+        <v>381</v>
+      </c>
+      <c r="B188" t="s">
+        <v>382</v>
+      </c>
+      <c r="C188" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="s">
+        <v>352</v>
+      </c>
+      <c r="B189" t="s">
+        <v>383</v>
+      </c>
+      <c r="C189" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="s">
+        <v>353</v>
+      </c>
+      <c r="B190" t="s">
+        <v>384</v>
+      </c>
+      <c r="C190" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" t="s">
+        <v>354</v>
+      </c>
+      <c r="B191" t="s">
+        <v>386</v>
+      </c>
+      <c r="C191" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" t="s">
+        <v>387</v>
+      </c>
+      <c r="B193" t="s">
+        <v>388</v>
+      </c>
+      <c r="C193" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" t="s">
+        <v>389</v>
+      </c>
+      <c r="B194" t="s">
+        <v>390</v>
+      </c>
+      <c r="C194" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" t="s">
+        <v>392</v>
+      </c>
+      <c r="B195" t="s">
+        <v>393</v>
+      </c>
+      <c r="C195" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" t="s">
+        <v>394</v>
+      </c>
+      <c r="B196" t="s">
+        <v>395</v>
+      </c>
+      <c r="C196" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" t="s">
+        <v>396</v>
+      </c>
+      <c r="B197" t="s">
+        <v>279</v>
+      </c>
+      <c r="C197" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" t="s">
+        <v>397</v>
+      </c>
+      <c r="B198" t="s">
+        <v>314</v>
+      </c>
+      <c r="C198" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" t="s">
+        <v>356</v>
+      </c>
+      <c r="B199" t="s">
+        <v>398</v>
+      </c>
+      <c r="C199" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" t="s">
+        <v>357</v>
+      </c>
+      <c r="B200" t="s">
+        <v>358</v>
+      </c>
+      <c r="C200" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" t="s">
+        <v>359</v>
+      </c>
+      <c r="B201" t="s">
+        <v>253</v>
+      </c>
+      <c r="C201" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" t="s">
+        <v>360</v>
+      </c>
+      <c r="B202" t="s">
+        <v>361</v>
+      </c>
+      <c r="C202" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" t="s">
+        <v>362</v>
+      </c>
+      <c r="B203" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" t="s">
+        <v>364</v>
+      </c>
+      <c r="B204" t="s">
+        <v>365</v>
+      </c>
+      <c r="C204" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" t="s">
+        <v>366</v>
+      </c>
+      <c r="B205" t="s">
+        <v>399</v>
+      </c>
+      <c r="C205" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" t="s">
+        <v>367</v>
+      </c>
+      <c r="B206" t="s">
+        <v>368</v>
+      </c>
+      <c r="C206" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" t="s">
+        <v>369</v>
+      </c>
+      <c r="B207" t="s">
+        <v>400</v>
+      </c>
+      <c r="C207" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" t="s">
+        <v>370</v>
+      </c>
+      <c r="B208" t="s">
+        <v>371</v>
+      </c>
+      <c r="C208" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" t="s">
+        <v>401</v>
+      </c>
+      <c r="B209" t="s">
+        <v>304</v>
+      </c>
+      <c r="C209" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" t="s">
+        <v>402</v>
+      </c>
+      <c r="B210" t="s">
+        <v>228</v>
+      </c>
+      <c r="C210" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>